<commit_message>
Updated recession lever files with May STEO data
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
+++ b/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
@@ -180,9 +180,6 @@
     <t>Recent 2020 Estimate</t>
   </si>
   <si>
-    <t>January 2020 and April 2020</t>
-  </si>
-  <si>
     <t>For the U.S. in EPS 2.1.1, we use EIA's 2020 projections from January 2020</t>
   </si>
   <si>
@@ -1042,6 +1039,9 @@
   </si>
   <si>
     <t>Impacts by Sector</t>
+  </si>
+  <si>
+    <t>January 2020 and May 2020</t>
   </si>
 </sst>
 </file>
@@ -1452,7 +1452,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:XFD29"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B4" s="21" t="s">
-        <v>47</v>
+        <v>334</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -1543,37 +1543,37 @@
     <row r="17" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="18" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
@@ -1587,13 +1587,13 @@
     </row>
     <row r="27" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B27"/>
     </row>
     <row r="28" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B28"/>
     </row>
@@ -1602,22 +1602,22 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -1636,7 +1636,7 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1652,14 +1652,14 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1680,12 +1680,12 @@
       </c>
       <c r="C4">
         <f>EIA!D5</f>
-        <v>-3.5940803382663845E-2</v>
+        <v>-5.9196617336152217E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B5" s="24">
         <f>SUM(BIFUbC!D3,BIFUbC!D13,BIFUbC!D23,BIFUbC!D33,BIFUbC!D43,BIFUbC!D53,BIFUbC!D63,BIFUbC!D73)/SUM(BIFUbC!D2:D81)</f>
@@ -1693,12 +1693,12 @@
       </c>
       <c r="C5">
         <f>EIA!I5</f>
-        <v>-5.2914427449359286E-2</v>
+        <v>-0.11740388590326579</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="24">
         <f>SUM(BIFUbC!D4,BIFUbC!D14,BIFUbC!D24,BIFUbC!D34,BIFUbC!D44,BIFUbC!D54,BIFUbC!D64,BIFUbC!D74)/SUM(BIFUbC!D2:D81)</f>
@@ -1706,12 +1706,12 @@
       </c>
       <c r="C6">
         <f>EIA!I11</f>
-        <v>-4.8951048951049021E-2</v>
+        <v>-9.0909090909090953E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -1724,12 +1724,12 @@
       </c>
       <c r="C9">
         <f>EIA!D3</f>
-        <v>-3.4989503149055285E-3</v>
+        <v>-9.0972708187543744E-3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="24">
         <v>0</v>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" s="24">
         <f>SUM(BCEU!D14:D19,BCEU!D74:D79)/SUM(BCEU!D2:D121)</f>
@@ -1748,12 +1748,12 @@
       </c>
       <c r="C11">
         <f>EIA!I3</f>
-        <v>-6.2454611474219275E-2</v>
+        <v>-3.9215686274509741E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -1766,12 +1766,12 @@
       </c>
       <c r="C14">
         <f>EIA!D4</f>
-        <v>-4.7232472324723246E-2</v>
+        <v>-6.494464944649446E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="24">
         <f>SUM(BCEU!D128:D133)/SUM(BCEU!D122:D181)</f>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16" s="24">
         <f>SUM(BCEU!D134:D139)/SUM(BCEU!D122:D181)</f>
@@ -1791,7 +1791,7 @@
       </c>
       <c r="C16">
         <f>EIA!I4</f>
-        <v>-5.2854122621564477E-2</v>
+        <v>-4.8625792811839409E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -1823,13 +1823,13 @@
       </c>
       <c r="C20">
         <f>EIA!C12</f>
-        <v>18693</v>
+        <v>18044</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="17">
         <f>-(1-C20/B20)</f>
-        <v>-3.882147264500202E-2</v>
+        <v>-7.2192513368983913E-2</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>31</v>
@@ -1867,23 +1867,23 @@
       </c>
       <c r="B26" s="6">
         <f>SUMPRODUCT(B9:B11,C9:C11)/SUM(B9:B11)</f>
-        <v>-3.2607755563336324E-2</v>
+        <v>-2.3967956222888956E-2</v>
       </c>
       <c r="C26" s="6">
         <f>SUMPRODUCT(B14:B16,C14:C16)/SUM(B14:B16)</f>
-        <v>-4.9448221252838979E-2</v>
+        <v>-5.7935659688453503E-2</v>
       </c>
       <c r="D26" s="6">
         <f>SUMPRODUCT(B4:B6,C4:C6)/SUM(B4:B6)</f>
-        <v>-4.6259161109703267E-2</v>
+        <v>-8.4996790026970415E-2</v>
       </c>
       <c r="E26" s="6">
         <f>(EIA!C10-EIA!B10)/EIA!B10</f>
-        <v>-9.3067110371602882E-2</v>
+        <v>-0.11259012756516916</v>
       </c>
       <c r="F26" s="14">
         <f>(EIA!C6-EIA!B6)/EIA!B6</f>
-        <v>-2.7027027027027029E-2</v>
+        <v>-4.3500643500643497E-2</v>
       </c>
       <c r="G26" s="14"/>
     </row>
@@ -1897,23 +1897,23 @@
       </c>
       <c r="B28" s="12">
         <f>B26/$A$22</f>
-        <v>0.83994123204737148</v>
+        <v>0.33200057879112871</v>
       </c>
       <c r="C28" s="12">
         <f>C26/$A$22</f>
-        <v>1.2737337840069052</v>
+        <v>0.80251617494376382</v>
       </c>
       <c r="D28" s="12">
         <f>D26/$A$22</f>
-        <v>1.1915869738563047</v>
+        <v>1.1773629433365538</v>
       </c>
       <c r="E28" s="12">
         <f>E26/$A$22</f>
-        <v>2.3973101490158073</v>
+        <v>1.5595817670138257</v>
       </c>
       <c r="F28" s="12">
         <f>F26/$A$22</f>
-        <v>0.69618757830678435</v>
+        <v>0.60256446923113627</v>
       </c>
       <c r="G28" s="15"/>
     </row>
@@ -1927,7 +1927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH181"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -1938,7 +1938,7 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1">
         <v>2018</v>
@@ -2042,7 +2042,7 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="23">
         <v>525200000000000</v>
@@ -2146,7 +2146,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="23">
         <v>585500000000000</v>
@@ -2250,7 +2250,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2354,7 +2354,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" s="23">
         <v>249600000000000</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="23">
         <v>1024000000000000</v>
@@ -2562,7 +2562,7 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="23">
         <v>1608000000000000</v>
@@ -2666,7 +2666,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2770,7 +2770,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2874,7 +2874,7 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3082,7 +3082,7 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="23">
         <v>2873000000000000</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="23">
         <v>50240000000000</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -3602,7 +3602,7 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3706,7 +3706,7 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="23">
         <v>910900000000000</v>
@@ -3810,7 +3810,7 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" s="23">
         <v>184500000000000</v>
@@ -3914,7 +3914,7 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B20" s="23">
         <v>332900000000000</v>
@@ -4018,7 +4018,7 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -4122,7 +4122,7 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -4226,7 +4226,7 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4330,7 +4330,7 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24" s="23">
         <v>42140000000000</v>
@@ -4434,7 +4434,7 @@
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B25" s="23">
         <v>6214000000000</v>
@@ -4538,7 +4538,7 @@
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -4642,7 +4642,7 @@
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -4746,7 +4746,7 @@
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -4850,7 +4850,7 @@
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4954,7 +4954,7 @@
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -5058,7 +5058,7 @@
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -5162,7 +5162,7 @@
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B32" s="23">
         <v>352000000000000</v>
@@ -5266,7 +5266,7 @@
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -5370,7 +5370,7 @@
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -5474,7 +5474,7 @@
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -5578,7 +5578,7 @@
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -5682,7 +5682,7 @@
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -5786,7 +5786,7 @@
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -5890,7 +5890,7 @@
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -5994,7 +5994,7 @@
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -6098,7 +6098,7 @@
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -6202,7 +6202,7 @@
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -6306,7 +6306,7 @@
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -6410,7 +6410,7 @@
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -6514,7 +6514,7 @@
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -6618,7 +6618,7 @@
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -6722,7 +6722,7 @@
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -6826,7 +6826,7 @@
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -6930,7 +6930,7 @@
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -7034,7 +7034,7 @@
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B50" s="23">
         <v>278900000000000</v>
@@ -7138,7 +7138,7 @@
     </row>
     <row r="51" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -7242,7 +7242,7 @@
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -7346,7 +7346,7 @@
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -7450,7 +7450,7 @@
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B54" s="23">
         <v>67490000000000</v>
@@ -7554,7 +7554,7 @@
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B55" s="23">
         <v>53540000000000</v>
@@ -7658,7 +7658,7 @@
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -7762,7 +7762,7 @@
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -7866,7 +7866,7 @@
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -7970,7 +7970,7 @@
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -8074,7 +8074,7 @@
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -8178,7 +8178,7 @@
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -8282,7 +8282,7 @@
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B62" s="23">
         <v>130300000000000</v>
@@ -8386,7 +8386,7 @@
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B63" s="23">
         <v>145300000000000</v>
@@ -8490,7 +8490,7 @@
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -8594,7 +8594,7 @@
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B65" s="23">
         <v>56950000000000</v>
@@ -8698,7 +8698,7 @@
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B66" s="23">
         <v>254200000000000</v>
@@ -8802,7 +8802,7 @@
     </row>
     <row r="67" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B67" s="23">
         <v>372400000000000</v>
@@ -8906,7 +8906,7 @@
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -9010,7 +9010,7 @@
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -9114,7 +9114,7 @@
     </row>
     <row r="70" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -9218,7 +9218,7 @@
     </row>
     <row r="71" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -9322,7 +9322,7 @@
     </row>
     <row r="72" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -9426,7 +9426,7 @@
     </row>
     <row r="73" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -9530,7 +9530,7 @@
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B74" s="23">
         <v>712900000000000</v>
@@ -9634,7 +9634,7 @@
     </row>
     <row r="75" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B75" s="23">
         <v>12470000000000</v>
@@ -9738,7 +9738,7 @@
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -9842,7 +9842,7 @@
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -9946,7 +9946,7 @@
     </row>
     <row r="78" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B78" s="23">
         <v>226000000000000</v>
@@ -10050,7 +10050,7 @@
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B79" s="23">
         <v>45780000000000</v>
@@ -10154,7 +10154,7 @@
     </row>
     <row r="80" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B80" s="23">
         <v>82600000000000</v>
@@ -10258,7 +10258,7 @@
     </row>
     <row r="81" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -10362,7 +10362,7 @@
     </row>
     <row r="82" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -10466,7 +10466,7 @@
     </row>
     <row r="83" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -10570,7 +10570,7 @@
     </row>
     <row r="84" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B84" s="23">
         <v>10460000000000</v>
@@ -10674,7 +10674,7 @@
     </row>
     <row r="85" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B85" s="23">
         <v>1542000000000</v>
@@ -10778,7 +10778,7 @@
     </row>
     <row r="86" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -10882,7 +10882,7 @@
     </row>
     <row r="87" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -10986,7 +10986,7 @@
     </row>
     <row r="88" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -11090,7 +11090,7 @@
     </row>
     <row r="89" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -11194,7 +11194,7 @@
     </row>
     <row r="90" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -11298,7 +11298,7 @@
     </row>
     <row r="91" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -11402,7 +11402,7 @@
     </row>
     <row r="92" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B92" s="23">
         <v>87350000000000</v>
@@ -11506,7 +11506,7 @@
     </row>
     <row r="93" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -11610,7 +11610,7 @@
     </row>
     <row r="94" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -11714,7 +11714,7 @@
     </row>
     <row r="95" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -11818,7 +11818,7 @@
     </row>
     <row r="96" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -11922,7 +11922,7 @@
     </row>
     <row r="97" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -12026,7 +12026,7 @@
     </row>
     <row r="98" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -12130,7 +12130,7 @@
     </row>
     <row r="99" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -12234,7 +12234,7 @@
     </row>
     <row r="100" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -12338,7 +12338,7 @@
     </row>
     <row r="101" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -12442,7 +12442,7 @@
     </row>
     <row r="102" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -12546,7 +12546,7 @@
     </row>
     <row r="103" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -12650,7 +12650,7 @@
     </row>
     <row r="104" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -12754,7 +12754,7 @@
     </row>
     <row r="105" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -12858,7 +12858,7 @@
     </row>
     <row r="106" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -12962,7 +12962,7 @@
     </row>
     <row r="107" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -13066,7 +13066,7 @@
     </row>
     <row r="108" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -13170,7 +13170,7 @@
     </row>
     <row r="109" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -13274,7 +13274,7 @@
     </row>
     <row r="110" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B110" s="23">
         <v>69201100000000</v>
@@ -13378,7 +13378,7 @@
     </row>
     <row r="111" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -13482,7 +13482,7 @@
     </row>
     <row r="112" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -13586,7 +13586,7 @@
     </row>
     <row r="113" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -13690,7 +13690,7 @@
     </row>
     <row r="114" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B114" s="23">
         <v>16747000000000</v>
@@ -13794,7 +13794,7 @@
     </row>
     <row r="115" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B115" s="23">
         <v>13287000000000</v>
@@ -13898,7 +13898,7 @@
     </row>
     <row r="116" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -14002,7 +14002,7 @@
     </row>
     <row r="117" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -14106,7 +14106,7 @@
     </row>
     <row r="118" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -14210,7 +14210,7 @@
     </row>
     <row r="119" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -14314,7 +14314,7 @@
     </row>
     <row r="120" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -14418,7 +14418,7 @@
     </row>
     <row r="121" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -14522,7 +14522,7 @@
     </row>
     <row r="122" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B122" s="23">
         <v>118600000000000</v>
@@ -14626,7 +14626,7 @@
     </row>
     <row r="123" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B123" s="23">
         <v>1023000000000000</v>
@@ -14730,7 +14730,7 @@
     </row>
     <row r="124" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -14834,7 +14834,7 @@
     </row>
     <row r="125" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B125" s="23">
         <v>481500000000000</v>
@@ -14938,7 +14938,7 @@
     </row>
     <row r="126" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B126" s="23">
         <v>761600000000000</v>
@@ -15042,7 +15042,7 @@
     </row>
     <row r="127" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B127" s="23">
         <v>2250000000000000</v>
@@ -15146,7 +15146,7 @@
     </row>
     <row r="128" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -15250,7 +15250,7 @@
     </row>
     <row r="129" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -15354,7 +15354,7 @@
     </row>
     <row r="130" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -15458,7 +15458,7 @@
     </row>
     <row r="131" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -15562,7 +15562,7 @@
     </row>
     <row r="132" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -15666,7 +15666,7 @@
     </row>
     <row r="133" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B133" s="23">
         <v>22590000000000</v>
@@ -15770,7 +15770,7 @@
     </row>
     <row r="134" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B134" s="23">
         <v>1848000000000000</v>
@@ -15874,7 +15874,7 @@
     </row>
     <row r="135" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B135" s="23">
         <v>28690000000000</v>
@@ -15978,7 +15978,7 @@
     </row>
     <row r="136" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -16082,7 +16082,7 @@
     </row>
     <row r="137" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -16186,7 +16186,7 @@
     </row>
     <row r="138" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B138" s="23">
         <v>936500000000000</v>
@@ -16290,7 +16290,7 @@
     </row>
     <row r="139" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B139" s="23">
         <v>606700000000000</v>
@@ -16394,7 +16394,7 @@
     </row>
     <row r="140" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B140" s="23">
         <v>232200000000000</v>
@@ -16498,7 +16498,7 @@
     </row>
     <row r="141" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -16602,7 +16602,7 @@
     </row>
     <row r="142" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -16706,7 +16706,7 @@
     </row>
     <row r="143" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -16810,7 +16810,7 @@
     </row>
     <row r="144" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B144" s="23">
         <v>6689000000000</v>
@@ -16914,7 +16914,7 @@
     </row>
     <row r="145" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B145" s="23">
         <v>106800000000000</v>
@@ -17018,7 +17018,7 @@
     </row>
     <row r="146" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B146" s="23">
         <v>375100000000000</v>
@@ -17122,7 +17122,7 @@
     </row>
     <row r="147" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -17226,7 +17226,7 @@
     </row>
     <row r="148" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -17330,7 +17330,7 @@
     </row>
     <row r="149" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -17434,7 +17434,7 @@
     </row>
     <row r="150" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -17538,7 +17538,7 @@
     </row>
     <row r="151" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -17642,7 +17642,7 @@
     </row>
     <row r="152" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -17746,7 +17746,7 @@
     </row>
     <row r="153" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -17850,7 +17850,7 @@
     </row>
     <row r="154" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -17954,7 +17954,7 @@
     </row>
     <row r="155" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -18058,7 +18058,7 @@
     </row>
     <row r="156" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -18162,7 +18162,7 @@
     </row>
     <row r="157" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -18266,7 +18266,7 @@
     </row>
     <row r="158" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -18370,7 +18370,7 @@
     </row>
     <row r="159" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -18474,7 +18474,7 @@
     </row>
     <row r="160" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -18578,7 +18578,7 @@
     </row>
     <row r="161" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -18682,7 +18682,7 @@
     </row>
     <row r="162" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -18786,7 +18786,7 @@
     </row>
     <row r="163" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -18890,7 +18890,7 @@
     </row>
     <row r="164" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -18994,7 +18994,7 @@
     </row>
     <row r="165" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -19098,7 +19098,7 @@
     </row>
     <row r="166" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -19202,7 +19202,7 @@
     </row>
     <row r="167" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -19306,7 +19306,7 @@
     </row>
     <row r="168" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -19410,7 +19410,7 @@
     </row>
     <row r="169" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -19514,7 +19514,7 @@
     </row>
     <row r="170" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B170" s="23">
         <v>364266000000000</v>
@@ -19618,7 +19618,7 @@
     </row>
     <row r="171" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -19722,7 +19722,7 @@
     </row>
     <row r="172" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -19826,7 +19826,7 @@
     </row>
     <row r="173" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -19930,7 +19930,7 @@
     </row>
     <row r="174" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B174" s="23">
         <v>10493400000000</v>
@@ -20034,7 +20034,7 @@
     </row>
     <row r="175" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B175" s="23">
         <v>167474000000000</v>
@@ -20138,7 +20138,7 @@
     </row>
     <row r="176" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -20242,7 +20242,7 @@
     </row>
     <row r="177" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -20346,7 +20346,7 @@
     </row>
     <row r="178" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -20450,7 +20450,7 @@
     </row>
     <row r="179" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -20554,7 +20554,7 @@
     </row>
     <row r="180" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -20658,7 +20658,7 @@
     </row>
     <row r="181" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -20780,7 +20780,7 @@
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1">
         <v>2018</v>
@@ -20884,7 +20884,7 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B2" s="23">
         <v>36840000000000</v>
@@ -20988,7 +20988,7 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B3" s="23">
         <v>178900000000000</v>
@@ -21092,7 +21092,7 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B4" s="23">
         <v>17370000000000</v>
@@ -21196,7 +21196,7 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -21300,7 +21300,7 @@
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B6" s="23">
         <v>51220000000000</v>
@@ -21404,7 +21404,7 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -21508,7 +21508,7 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -21612,7 +21612,7 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B9" s="23">
         <v>7244910000000</v>
@@ -21716,7 +21716,7 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B10" s="23">
         <v>802708000000</v>
@@ -21820,7 +21820,7 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -21924,7 +21924,7 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B12" s="23">
         <v>237800000000000</v>
@@ -22028,7 +22028,7 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B13" s="23">
         <v>24000000000000</v>
@@ -22132,7 +22132,7 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B14" s="23">
         <v>4107000000000000</v>
@@ -22236,7 +22236,7 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B15" s="23">
         <v>782400000000000</v>
@@ -22340,7 +22340,7 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -22444,7 +22444,7 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -22548,7 +22548,7 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B18" s="23">
         <v>3.77021E+16</v>
@@ -22652,7 +22652,7 @@
     </row>
     <row r="19" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -22756,7 +22756,7 @@
     </row>
     <row r="20" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -22860,7 +22860,7 @@
     </row>
     <row r="21" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -22964,7 +22964,7 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B22" s="23">
         <v>212900000000000</v>
@@ -23068,7 +23068,7 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B23" s="23">
         <v>79170000000000</v>
@@ -23172,7 +23172,7 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B24" s="23">
         <v>426800000000000</v>
@@ -23276,7 +23276,7 @@
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -23380,7 +23380,7 @@
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B26" s="23">
         <v>2610000000000</v>
@@ -23484,7 +23484,7 @@
     </row>
     <row r="27" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -23588,7 +23588,7 @@
     </row>
     <row r="28" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -23692,7 +23692,7 @@
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B29" s="23">
         <v>28794600000000</v>
@@ -23796,7 +23796,7 @@
     </row>
     <row r="30" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B30" s="23">
         <v>401983000000</v>
@@ -23900,7 +23900,7 @@
     </row>
     <row r="31" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -24004,7 +24004,7 @@
     </row>
     <row r="32" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B32" s="23">
         <v>415200000000000</v>
@@ -24108,7 +24108,7 @@
     </row>
     <row r="33" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B33" s="23">
         <v>51750000000000</v>
@@ -24212,7 +24212,7 @@
     </row>
     <row r="34" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B34" s="23">
         <v>3314000000000000</v>
@@ -24316,7 +24316,7 @@
     </row>
     <row r="35" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -24420,7 +24420,7 @@
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B36" s="23">
         <v>68090000000000</v>
@@ -24524,7 +24524,7 @@
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -24628,7 +24628,7 @@
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -24732,7 +24732,7 @@
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B39" s="23">
         <v>174878000000000</v>
@@ -24836,7 +24836,7 @@
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B40" s="23">
         <v>3253690000000000</v>
@@ -24940,7 +24940,7 @@
     </row>
     <row r="41" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -25044,7 +25044,7 @@
     </row>
     <row r="42" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B42" s="23">
         <v>83110000000000</v>
@@ -25148,7 +25148,7 @@
     </row>
     <row r="43" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B43" s="23">
         <v>88130000000000</v>
@@ -25252,7 +25252,7 @@
     </row>
     <row r="44" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B44" s="23">
         <v>61250000000000</v>
@@ -25356,7 +25356,7 @@
     </row>
     <row r="45" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -25460,7 +25460,7 @@
     </row>
     <row r="46" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B46" s="23">
         <v>74690000000000</v>
@@ -25564,7 +25564,7 @@
     </row>
     <row r="47" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -25668,7 +25668,7 @@
     </row>
     <row r="48" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -25772,7 +25772,7 @@
     </row>
     <row r="49" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B49" s="23">
         <v>18922700000000</v>
@@ -25876,7 +25876,7 @@
     </row>
     <row r="50" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -25980,7 +25980,7 @@
     </row>
     <row r="51" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -26084,7 +26084,7 @@
     </row>
     <row r="52" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B52" s="23">
         <v>221000000000000</v>
@@ -26188,7 +26188,7 @@
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -26292,7 +26292,7 @@
     </row>
     <row r="54" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -26396,7 +26396,7 @@
     </row>
     <row r="55" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -26500,7 +26500,7 @@
     </row>
     <row r="56" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -26604,7 +26604,7 @@
     </row>
     <row r="57" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -26708,7 +26708,7 @@
     </row>
     <row r="58" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -26812,7 +26812,7 @@
     </row>
     <row r="59" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -26916,7 +26916,7 @@
     </row>
     <row r="60" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -27020,7 +27020,7 @@
     </row>
     <row r="61" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -27124,7 +27124,7 @@
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B62" s="23">
         <v>153700000000000</v>
@@ -27228,7 +27228,7 @@
     </row>
     <row r="63" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -27332,7 +27332,7 @@
     </row>
     <row r="64" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B64" s="23">
         <v>68730000000000</v>
@@ -27436,7 +27436,7 @@
     </row>
     <row r="65" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -27540,7 +27540,7 @@
     </row>
     <row r="66" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B66" s="23">
         <v>575400000000000</v>
@@ -27644,7 +27644,7 @@
     </row>
     <row r="67" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -27748,7 +27748,7 @@
     </row>
     <row r="68" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -27852,7 +27852,7 @@
     </row>
     <row r="69" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B69" s="23">
         <v>68400000000000</v>
@@ -27956,7 +27956,7 @@
     </row>
     <row r="70" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B70" s="23">
         <v>208675000000000</v>
@@ -28060,7 +28060,7 @@
     </row>
     <row r="71" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -28164,7 +28164,7 @@
     </row>
     <row r="72" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B72" s="23">
         <v>1877000000000000</v>
@@ -28268,7 +28268,7 @@
     </row>
     <row r="73" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B73" s="23">
         <v>163700000000000</v>
@@ -28372,7 +28372,7 @@
     </row>
     <row r="74" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B74" s="23">
         <v>3050000000000000</v>
@@ -28476,7 +28476,7 @@
     </row>
     <row r="75" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -28580,7 +28580,7 @@
     </row>
     <row r="76" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B76" s="23">
         <v>2191000000000000</v>
@@ -28684,7 +28684,7 @@
     </row>
     <row r="77" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -28788,7 +28788,7 @@
     </row>
     <row r="78" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -28892,7 +28892,7 @@
     </row>
     <row r="79" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B79" s="23">
         <v>229496000000000</v>
@@ -28996,7 +28996,7 @@
     </row>
     <row r="80" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B80" s="23">
         <v>289305000000000</v>
@@ -29100,7 +29100,7 @@
     </row>
     <row r="81" spans="1:34" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -29212,7 +29212,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection sqref="A1:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29229,7 +29229,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="F1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -29237,7 +29237,7 @@
     </row>
     <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A2" s="20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>45</v>
@@ -29249,7 +29249,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G2" s="20" t="s">
         <v>45</v>
@@ -29269,11 +29269,11 @@
         <v>1429</v>
       </c>
       <c r="C3">
-        <v>1424</v>
+        <v>1416</v>
       </c>
       <c r="D3">
         <f>(C3-B3)/B3</f>
-        <v>-3.4989503149055285E-3</v>
+        <v>-9.0972708187543744E-3</v>
       </c>
       <c r="F3" t="s">
         <v>35</v>
@@ -29282,11 +29282,11 @@
         <v>13.77</v>
       </c>
       <c r="H3">
-        <v>12.91</v>
+        <v>13.23</v>
       </c>
       <c r="I3">
         <f>(H3-G3)/G3</f>
-        <v>-6.2454611474219275E-2</v>
+        <v>-3.9215686274509741E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -29297,11 +29297,11 @@
         <v>1355</v>
       </c>
       <c r="C4">
-        <v>1291</v>
+        <v>1267</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D6" si="0">(C4-B4)/B4</f>
-        <v>-4.7232472324723246E-2</v>
+        <v>-6.494464944649446E-2</v>
       </c>
       <c r="F4" t="s">
         <v>36</v>
@@ -29310,11 +29310,11 @@
         <v>9.4600000000000009</v>
       </c>
       <c r="H4">
-        <v>8.9600000000000009</v>
+        <v>9</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I5" si="1">(H4-G4)/G4</f>
-        <v>-5.2854122621564477E-2</v>
+        <v>-4.8625792811839409E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -29325,11 +29325,11 @@
         <v>946</v>
       </c>
       <c r="C5">
-        <v>912</v>
+        <v>890</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>-3.5940803382663845E-2</v>
+        <v>-5.9196617336152217E-2</v>
       </c>
       <c r="F5" t="s">
         <v>37</v>
@@ -29338,11 +29338,11 @@
         <v>24.19</v>
       </c>
       <c r="H5">
-        <v>22.91</v>
+        <v>21.35</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>-5.2914427449359286E-2</v>
+        <v>-0.11740388590326579</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -29353,11 +29353,11 @@
         <v>3885</v>
       </c>
       <c r="C6">
-        <v>3780</v>
+        <v>3716</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-2.7027027027027029E-2</v>
+        <v>-4.3500643500643497E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -29368,7 +29368,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -29385,7 +29385,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G9" s="20" t="s">
         <v>45</v>
@@ -29405,39 +29405,39 @@
         <v>9015</v>
       </c>
       <c r="C10">
-        <v>8176</v>
+        <v>8000</v>
       </c>
       <c r="D10">
         <f>(C10-B10)/B10</f>
-        <v>-9.3067110371602882E-2</v>
+        <v>-0.11259012756516916</v>
       </c>
       <c r="F10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10">
         <v>0.7</v>
       </c>
       <c r="H10">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <f>(H10-G10)/G10</f>
-        <v>0.28571428571428581</v>
+        <v>0.42857142857142866</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11">
         <v>28.6</v>
       </c>
       <c r="H11">
-        <v>27.2</v>
+        <v>26</v>
       </c>
       <c r="I11">
         <f>(H11-G11)/G11</f>
-        <v>-4.8951048951049021E-2</v>
+        <v>-9.0909090909090953E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -29448,11 +29448,11 @@
         <v>19448</v>
       </c>
       <c r="C12">
-        <v>18693</v>
+        <v>18044</v>
       </c>
       <c r="D12">
         <f>(C12-B12)/B12</f>
-        <v>-3.8821472645002054E-2</v>
+        <v>-7.2192513368983954E-2</v>
       </c>
     </row>
   </sheetData>
@@ -29490,7 +29490,7 @@
       </c>
       <c r="B2" s="7">
         <f>Calculations!E28</f>
-        <v>2.3973101490158073</v>
+        <v>1.5595817670138257</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -29499,7 +29499,7 @@
       </c>
       <c r="B3" s="15">
         <f>Calculations!F28</f>
-        <v>0.69618757830678435</v>
+        <v>0.60256446923113627</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -29508,7 +29508,7 @@
       </c>
       <c r="B4" s="7">
         <f>Calculations!B28</f>
-        <v>0.83994123204737148</v>
+        <v>0.33200057879112871</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -29517,7 +29517,7 @@
       </c>
       <c r="B5" s="7">
         <f>Calculations!C28</f>
-        <v>1.2737337840069052</v>
+        <v>0.80251617494376382</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -29526,7 +29526,7 @@
       </c>
       <c r="B6" s="7">
         <f>Calculations!D28</f>
-        <v>1.1915869738563047</v>
+        <v>1.1773629433365538</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Updated recession files for September STEO and CBO projections on recovery timeline.
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
+++ b/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
@@ -19,7 +19,7 @@
     <sheet name="EIA" sheetId="8" r:id="rId5"/>
     <sheet name="EoSEUwGDPiR" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -165,9 +165,6 @@
     <t>https://www.eia.gov/outlooks/steo/</t>
   </si>
   <si>
-    <t>Tables 7a and 9a</t>
-  </si>
-  <si>
     <t>The EIA Short-Term Energy Outlook does not include total energy demand by</t>
   </si>
   <si>
@@ -1041,10 +1038,13 @@
     <t>Note that the Electricity Sector energy use multiplier is only used to adjust imports and exports of electricity and of certain fuels used by the electricity sector. Changes in domestic electricity demand are derived from the buildings, transport, and industry sectors' multipliers.</t>
   </si>
   <si>
-    <t>January 2020 and July 2020</t>
-  </si>
-  <si>
     <t>Additional data from EPS variables bldgs/BCEU and indst/BIFUbC</t>
+  </si>
+  <si>
+    <t>January 2020 and September 2020</t>
+  </si>
+  <si>
+    <t>Tables 5a, 6, 7a, and 9a</t>
   </si>
 </sst>
 </file>
@@ -1458,7 +1458,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1496,12 +1496,12 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>42</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="21" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
@@ -1554,37 +1554,37 @@
     <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
@@ -1592,19 +1592,19 @@
     </row>
     <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30"/>
     </row>
     <row r="31" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B31"/>
     </row>
     <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B32"/>
     </row>
@@ -1613,22 +1613,22 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -1647,7 +1647,7 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1664,14 +1664,14 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B2" s="19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -1692,12 +1692,12 @@
       </c>
       <c r="C4">
         <f>EIA!D5</f>
-        <v>-4.9682875264270614E-2</v>
+        <v>-5.3911205073995772E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="23">
         <f>SUM(BIFUbC!C3,BIFUbC!C13,BIFUbC!C23,BIFUbC!C33,BIFUbC!C43,BIFUbC!C53,BIFUbC!C63,BIFUbC!C73)/SUM(BIFUbC!C2:C81)</f>
@@ -1705,12 +1705,12 @@
       </c>
       <c r="C5">
         <f>EIA!I5</f>
-        <v>-0.10913600661430345</v>
+        <v>-9.2600248036378743E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="23">
         <f>SUM(BIFUbC!C4,BIFUbC!C14,BIFUbC!C24,BIFUbC!C34,BIFUbC!C44,BIFUbC!C54,BIFUbC!C64,BIFUbC!C74)/SUM(BIFUbC!C2:C81)</f>
@@ -1718,12 +1718,12 @@
       </c>
       <c r="C6">
         <f>EIA!I11</f>
-        <v>-8.0419580419580444E-2</v>
+        <v>-9.4405594405594498E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
@@ -1736,12 +1736,12 @@
       </c>
       <c r="C9">
         <f>EIA!D3</f>
-        <v>4.1987403778866337E-3</v>
+        <v>3.9188243526941918E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="23">
         <v>0</v>
@@ -1752,7 +1752,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" s="23">
         <f>SUM(BCEU!C14:C19,BCEU!C74:C79)/SUM(BCEU!C2:C121)</f>
@@ -1760,12 +1760,12 @@
       </c>
       <c r="C11">
         <f>EIA!I3</f>
-        <v>-7.2621641249092234E-2</v>
+        <v>-6.1728395061728371E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -1774,20 +1774,20 @@
       </c>
       <c r="B14" s="23">
         <f>SUM(BCEU!C122:C127)/SUM(BCEU!C122:C181)</f>
-        <v>0.49371765159146319</v>
+        <v>0.49352918272424123</v>
       </c>
       <c r="C14">
         <f>EIA!D4</f>
-        <v>-7.0110701107011064E-2</v>
+        <v>-6.4206642066420669E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="23">
         <f>SUM(BCEU!C128:C133)/SUM(BCEU!C122:C181)</f>
-        <v>2.3432574014686253E-3</v>
+        <v>2.3423629001951933E-3</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1795,15 +1795,15 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" s="23">
         <f>SUM(BCEU!C134:C139)/SUM(BCEU!C122:C181)</f>
-        <v>0.3770363744832953</v>
+        <v>0.37689244683928402</v>
       </c>
       <c r="C16">
         <f>EIA!I4</f>
-        <v>-4.8625792811839409E-2</v>
+        <v>-6.9767441860465129E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -1835,13 +1835,13 @@
       </c>
       <c r="C20">
         <f>EIA!C12</f>
-        <v>17517</v>
+        <v>18168</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="16">
         <f>-(1-C20/B20)</f>
-        <v>-9.9290415466886106E-2</v>
+        <v>-6.5816536404771697E-2</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>30</v>
@@ -1870,7 +1870,7 @@
         <v>5</v>
       </c>
       <c r="G25" s="25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -1879,23 +1879,23 @@
       </c>
       <c r="B26" s="6">
         <f>SUMPRODUCT(B9:B11,C9:C11)/SUM(B9:B11)</f>
-        <v>-3.5358901544302969E-2</v>
+        <v>-1.2777447982714234E-2</v>
       </c>
       <c r="C26" s="6">
         <f>SUMPRODUCT(B14:B16,C14:C16)/SUM(B14:B16)</f>
-        <v>-6.0644540227318217E-2</v>
+        <v>-6.643568474145882E-2</v>
       </c>
       <c r="D26" s="6">
         <f>SUMPRODUCT(B4:B6,C4:C6)/SUM(B4:B6)</f>
-        <v>-7.6111241595777548E-2</v>
+        <v>-8.6111701307997141E-2</v>
       </c>
       <c r="E26" s="6">
         <f>(EIA!C10-EIA!B10)/EIA!B10</f>
-        <v>-0.12024403771491958</v>
+        <v>-0.12656683305601774</v>
       </c>
       <c r="F26" s="13">
         <f>(EIA!C6-EIA!B6)/EIA!B6</f>
-        <v>-3.9897039897039896E-2</v>
+        <v>-2.1364221364221364E-2</v>
       </c>
       <c r="G26" s="24"/>
     </row>
@@ -1909,23 +1909,23 @@
       </c>
       <c r="B28" s="11">
         <f>B26/$A$22</f>
-        <v>0.35611595920953071</v>
+        <v>0.1941373502873644</v>
       </c>
       <c r="C28" s="11">
         <f>C26/$A$22</f>
-        <v>0.61077939841578666</v>
+        <v>1.0094071850405399</v>
       </c>
       <c r="D28" s="11">
         <f>D26/$A$22</f>
-        <v>0.76655174860418485</v>
+        <v>1.3083596617483817</v>
       </c>
       <c r="E28" s="11">
         <f>E26/$A$22</f>
-        <v>1.2110336848678172</v>
+        <v>1.9230248197448696</v>
       </c>
       <c r="F28" s="11">
         <f>F26/$A$22</f>
-        <v>0.40182166334419034</v>
+        <v>0.32460263835263836</v>
       </c>
       <c r="G28" s="14"/>
     </row>
@@ -1939,15 +1939,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG181"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView topLeftCell="A160" workbookViewId="0">
+      <selection sqref="A1:AG181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="23.53125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1">
         <v>2019</v>
@@ -2048,7 +2051,7 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A2" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="22">
         <v>570800000000000</v>
@@ -2149,7 +2152,7 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="22">
         <v>688800000000000</v>
@@ -2250,7 +2253,7 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2351,7 +2354,7 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A5" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B5" s="22">
         <v>205100000000000</v>
@@ -2452,7 +2455,7 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A6" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="22">
         <v>1025000000000000</v>
@@ -2553,7 +2556,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A7" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B7" s="22">
         <v>1437000000000000</v>
@@ -2654,7 +2657,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2755,7 +2758,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2856,7 +2859,7 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2957,7 +2960,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -3058,7 +3061,7 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3159,7 +3162,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -3260,7 +3263,7 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A14" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="22">
         <v>3041000000000000</v>
@@ -3361,7 +3364,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A15" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="22">
         <v>48530000000000</v>
@@ -3462,7 +3465,7 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -3563,7 +3566,7 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3664,7 +3667,7 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A18" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" s="22">
         <v>912300000000000</v>
@@ -3765,7 +3768,7 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A19" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="22">
         <v>184400000000000</v>
@@ -3866,7 +3869,7 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A20" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" s="22">
         <v>317500000000000</v>
@@ -3967,7 +3970,7 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -4068,7 +4071,7 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -4169,7 +4172,7 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4270,7 +4273,7 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A24" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B24" s="22">
         <v>39890000000000</v>
@@ -4371,7 +4374,7 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A25" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B25" s="22">
         <v>6120000000000</v>
@@ -4472,7 +4475,7 @@
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -4573,7 +4576,7 @@
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -4674,7 +4677,7 @@
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -4775,7 +4778,7 @@
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4876,7 +4879,7 @@
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -4977,7 +4980,7 @@
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -5078,7 +5081,7 @@
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A32" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B32" s="22">
         <v>423700000000000</v>
@@ -5179,7 +5182,7 @@
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -5280,7 +5283,7 @@
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -5381,7 +5384,7 @@
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -5482,7 +5485,7 @@
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -5583,7 +5586,7 @@
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -5684,7 +5687,7 @@
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -5785,7 +5788,7 @@
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -5886,7 +5889,7 @@
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -5987,7 +5990,7 @@
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -6088,7 +6091,7 @@
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -6189,7 +6192,7 @@
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -6290,7 +6293,7 @@
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -6391,7 +6394,7 @@
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -6492,7 +6495,7 @@
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -6593,7 +6596,7 @@
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -6694,7 +6697,7 @@
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -6795,7 +6798,7 @@
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -6896,7 +6899,7 @@
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A50" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B50" s="22">
         <v>250300000000000</v>
@@ -6997,7 +7000,7 @@
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -7098,7 +7101,7 @@
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -7199,7 +7202,7 @@
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -7300,7 +7303,7 @@
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A54" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B54" s="22">
         <v>65490000000000</v>
@@ -7401,7 +7404,7 @@
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A55" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B55" s="22">
         <v>54350000000000</v>
@@ -7502,7 +7505,7 @@
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -7603,7 +7606,7 @@
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -7704,7 +7707,7 @@
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -7805,7 +7808,7 @@
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -7906,7 +7909,7 @@
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -8007,7 +8010,7 @@
     </row>
     <row r="61" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -8108,7 +8111,7 @@
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A62" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B62" s="22">
         <v>141600000000000</v>
@@ -8209,7 +8212,7 @@
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A63" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B63" s="22">
         <v>170900000000000</v>
@@ -8310,7 +8313,7 @@
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -8411,7 +8414,7 @@
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A65" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B65" s="22">
         <v>50910000000000</v>
@@ -8512,7 +8515,7 @@
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A66" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B66" s="22">
         <v>254400000000000</v>
@@ -8613,7 +8616,7 @@
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A67" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B67" s="22">
         <v>356600000000000</v>
@@ -8714,7 +8717,7 @@
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -8815,7 +8818,7 @@
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -8916,7 +8919,7 @@
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -9017,7 +9020,7 @@
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -9118,7 +9121,7 @@
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -9219,7 +9222,7 @@
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -9320,7 +9323,7 @@
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A74" s="22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B74" s="22">
         <v>754700000000000</v>
@@ -9421,7 +9424,7 @@
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A75" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B75" s="22">
         <v>12040000000000</v>
@@ -9522,7 +9525,7 @@
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -9623,7 +9626,7 @@
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -9724,7 +9727,7 @@
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A78" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B78" s="22">
         <v>226400000000000</v>
@@ -9825,7 +9828,7 @@
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A79" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B79" s="22">
         <v>45750000000000</v>
@@ -9926,7 +9929,7 @@
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A80" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B80" s="22">
         <v>78790000000000</v>
@@ -10027,7 +10030,7 @@
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -10128,7 +10131,7 @@
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -10229,7 +10232,7 @@
     </row>
     <row r="83" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -10330,7 +10333,7 @@
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A84" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B84" s="22">
         <v>9900000000000</v>
@@ -10431,7 +10434,7 @@
     </row>
     <row r="85" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A85" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B85" s="22">
         <v>1519000000000</v>
@@ -10532,7 +10535,7 @@
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -10633,7 +10636,7 @@
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -10734,7 +10737,7 @@
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -10835,7 +10838,7 @@
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -10936,7 +10939,7 @@
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -11037,7 +11040,7 @@
     </row>
     <row r="91" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -11138,7 +11141,7 @@
     </row>
     <row r="92" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A92" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B92" s="22">
         <v>105100000000000</v>
@@ -11239,7 +11242,7 @@
     </row>
     <row r="93" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -11340,7 +11343,7 @@
     </row>
     <row r="94" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -11441,7 +11444,7 @@
     </row>
     <row r="95" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -11542,7 +11545,7 @@
     </row>
     <row r="96" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -11643,7 +11646,7 @@
     </row>
     <row r="97" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -11744,7 +11747,7 @@
     </row>
     <row r="98" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -11845,7 +11848,7 @@
     </row>
     <row r="99" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -11946,7 +11949,7 @@
     </row>
     <row r="100" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -12047,7 +12050,7 @@
     </row>
     <row r="101" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -12148,7 +12151,7 @@
     </row>
     <row r="102" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -12249,7 +12252,7 @@
     </row>
     <row r="103" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -12350,7 +12353,7 @@
     </row>
     <row r="104" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -12451,7 +12454,7 @@
     </row>
     <row r="105" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -12552,7 +12555,7 @@
     </row>
     <row r="106" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -12653,7 +12656,7 @@
     </row>
     <row r="107" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -12754,7 +12757,7 @@
     </row>
     <row r="108" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -12855,7 +12858,7 @@
     </row>
     <row r="109" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -12956,7 +12959,7 @@
     </row>
     <row r="110" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A110" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B110" s="22">
         <v>62110000000000</v>
@@ -13057,7 +13060,7 @@
     </row>
     <row r="111" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -13158,7 +13161,7 @@
     </row>
     <row r="112" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -13259,7 +13262,7 @@
     </row>
     <row r="113" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -13360,7 +13363,7 @@
     </row>
     <row r="114" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A114" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B114" s="22">
         <v>16250000000000</v>
@@ -13461,7 +13464,7 @@
     </row>
     <row r="115" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A115" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B115" s="22">
         <v>13490000000000</v>
@@ -13562,7 +13565,7 @@
     </row>
     <row r="116" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -13663,7 +13666,7 @@
     </row>
     <row r="117" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -13764,7 +13767,7 @@
     </row>
     <row r="118" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -13865,7 +13868,7 @@
     </row>
     <row r="119" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -13966,7 +13969,7 @@
     </row>
     <row r="120" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -14067,7 +14070,7 @@
     </row>
     <row r="121" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -14168,7 +14171,7 @@
     </row>
     <row r="122" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A122" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B122" s="22">
         <v>123700000000000</v>
@@ -14269,7 +14272,7 @@
     </row>
     <row r="123" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A123" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B123" s="22">
         <v>1042000000000000</v>
@@ -14370,7 +14373,7 @@
     </row>
     <row r="124" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -14471,7 +14474,7 @@
     </row>
     <row r="125" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A125" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B125" s="22">
         <v>482000000000000</v>
@@ -14572,7 +14575,7 @@
     </row>
     <row r="126" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A126" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B126" s="22">
         <v>771000000000000</v>
@@ -14673,7 +14676,7 @@
     </row>
     <row r="127" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A127" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B127" s="22">
         <v>2236000000000000</v>
@@ -14774,7 +14777,7 @@
     </row>
     <row r="128" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -14875,7 +14878,7 @@
     </row>
     <row r="129" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -14976,7 +14979,7 @@
     </row>
     <row r="130" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -15077,7 +15080,7 @@
     </row>
     <row r="131" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -15178,7 +15181,7 @@
     </row>
     <row r="132" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -15279,7 +15282,7 @@
     </row>
     <row r="133" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A133" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B133" s="22">
         <v>21730000000000</v>
@@ -15380,7 +15383,7 @@
     </row>
     <row r="134" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A134" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B134" s="22">
         <v>1882000000000000</v>
@@ -15481,7 +15484,7 @@
     </row>
     <row r="135" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A135" s="22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B135" s="22">
         <v>27450000000000</v>
@@ -15582,7 +15585,7 @@
     </row>
     <row r="136" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -15683,7 +15686,7 @@
     </row>
     <row r="137" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -15784,7 +15787,7 @@
     </row>
     <row r="138" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A138" s="22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B138" s="22">
         <v>951100000000000</v>
@@ -15885,7 +15888,7 @@
     </row>
     <row r="139" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A139" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B139" s="22">
         <v>774500000000000</v>
@@ -15986,7 +15989,7 @@
     </row>
     <row r="140" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A140" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B140" s="22">
         <v>226700000000000</v>
@@ -16087,7 +16090,7 @@
     </row>
     <row r="141" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -16188,7 +16191,7 @@
     </row>
     <row r="142" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -16289,7 +16292,7 @@
     </row>
     <row r="143" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -16390,7 +16393,7 @@
     </row>
     <row r="144" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A144" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B144" s="22">
         <v>6466000000000</v>
@@ -16491,7 +16494,7 @@
     </row>
     <row r="145" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A145" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B145" s="22">
         <v>104000000000000</v>
@@ -16592,108 +16595,108 @@
     </row>
     <row r="146" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A146" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B146" s="22">
+        <v>336400000000000</v>
+      </c>
+      <c r="C146" s="22">
+        <v>331900000000000</v>
+      </c>
+      <c r="D146" s="22">
         <v>328300000000000</v>
       </c>
-      <c r="C146" s="22">
+      <c r="E146" s="22">
         <v>328300000000000</v>
       </c>
-      <c r="D146" s="22">
+      <c r="F146" s="22">
         <v>327700000000000</v>
       </c>
-      <c r="E146" s="22">
+      <c r="G146" s="22">
         <v>326800000000000</v>
       </c>
-      <c r="F146" s="22">
+      <c r="H146" s="22">
         <v>325000000000000</v>
       </c>
-      <c r="G146" s="22">
+      <c r="I146" s="22">
         <v>323000000000000</v>
       </c>
-      <c r="H146" s="22">
+      <c r="J146" s="22">
         <v>321300000000000</v>
       </c>
-      <c r="I146" s="22">
+      <c r="K146" s="22">
         <v>320000000000000</v>
       </c>
-      <c r="J146" s="22">
+      <c r="L146" s="22">
         <v>319200000000000</v>
       </c>
-      <c r="K146" s="22">
+      <c r="M146" s="22">
         <v>318500000000000</v>
       </c>
-      <c r="L146" s="22">
+      <c r="N146" s="22">
         <v>318200000000000</v>
       </c>
-      <c r="M146" s="22">
+      <c r="O146" s="22">
         <v>318000000000000</v>
       </c>
-      <c r="N146" s="22">
+      <c r="P146" s="22">
         <v>317500000000000</v>
       </c>
-      <c r="O146" s="22">
+      <c r="Q146" s="22">
         <v>316800000000000</v>
       </c>
-      <c r="P146" s="22">
+      <c r="R146" s="22">
         <v>316400000000000</v>
       </c>
-      <c r="Q146" s="22">
+      <c r="S146" s="22">
         <v>316300000000000</v>
       </c>
-      <c r="R146" s="22">
+      <c r="T146" s="22">
         <v>315900000000000</v>
       </c>
-      <c r="S146" s="22">
+      <c r="U146" s="22">
         <v>315500000000000</v>
       </c>
-      <c r="T146" s="22">
+      <c r="V146" s="22">
         <v>315200000000000</v>
       </c>
-      <c r="U146" s="22">
+      <c r="W146" s="22">
         <v>315000000000000</v>
       </c>
-      <c r="V146" s="22">
+      <c r="X146" s="22">
         <v>314800000000000</v>
       </c>
-      <c r="W146" s="22">
+      <c r="Y146" s="22">
         <v>314600000000000</v>
       </c>
-      <c r="X146" s="22">
+      <c r="Z146" s="22">
         <v>314400000000000</v>
       </c>
-      <c r="Y146" s="22">
+      <c r="AA146" s="22">
         <v>314300000000000</v>
       </c>
-      <c r="Z146" s="22">
+      <c r="AB146" s="22">
         <v>314200000000000</v>
       </c>
-      <c r="AA146" s="22">
+      <c r="AC146" s="22">
         <v>314000000000000</v>
       </c>
-      <c r="AB146" s="22">
+      <c r="AD146" s="22">
         <v>313800000000000</v>
       </c>
-      <c r="AC146" s="22">
+      <c r="AE146" s="22">
         <v>313700000000000</v>
       </c>
-      <c r="AD146" s="22">
+      <c r="AF146" s="22">
         <v>313600000000000</v>
       </c>
-      <c r="AE146" s="22">
+      <c r="AG146" s="22">
         <v>313500000000000</v>
-      </c>
-      <c r="AF146" s="22">
-        <v>-342200000000</v>
-      </c>
-      <c r="AG146" s="22">
-        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -16794,7 +16797,7 @@
     </row>
     <row r="148" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -16895,7 +16898,7 @@
     </row>
     <row r="149" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -16996,7 +16999,7 @@
     </row>
     <row r="150" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -17097,7 +17100,7 @@
     </row>
     <row r="151" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -17198,7 +17201,7 @@
     </row>
     <row r="152" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -17299,7 +17302,7 @@
     </row>
     <row r="153" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -17400,7 +17403,7 @@
     </row>
     <row r="154" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -17501,7 +17504,7 @@
     </row>
     <row r="155" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B155">
         <v>0</v>
@@ -17602,7 +17605,7 @@
     </row>
     <row r="156" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -17703,7 +17706,7 @@
     </row>
     <row r="157" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -17804,7 +17807,7 @@
     </row>
     <row r="158" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -17905,7 +17908,7 @@
     </row>
     <row r="159" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -18006,7 +18009,7 @@
     </row>
     <row r="160" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -18107,7 +18110,7 @@
     </row>
     <row r="161" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -18208,7 +18211,7 @@
     </row>
     <row r="162" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -18309,7 +18312,7 @@
     </row>
     <row r="163" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -18410,7 +18413,7 @@
     </row>
     <row r="164" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -18511,7 +18514,7 @@
     </row>
     <row r="165" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -18612,7 +18615,7 @@
     </row>
     <row r="166" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -18713,7 +18716,7 @@
     </row>
     <row r="167" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B167">
         <v>0</v>
@@ -18814,7 +18817,7 @@
     </row>
     <row r="168" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -18915,7 +18918,7 @@
     </row>
     <row r="169" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -19016,7 +19019,7 @@
     </row>
     <row r="170" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A170" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B170" s="22">
         <v>350500000000000</v>
@@ -19117,7 +19120,7 @@
     </row>
     <row r="171" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B171">
         <v>0</v>
@@ -19218,7 +19221,7 @@
     </row>
     <row r="172" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -19319,7 +19322,7 @@
     </row>
     <row r="173" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -19420,7 +19423,7 @@
     </row>
     <row r="174" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A174" s="22" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B174" s="22">
         <v>10000000000000</v>
@@ -19521,7 +19524,7 @@
     </row>
     <row r="175" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A175" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B175" s="22">
         <v>160900000000000</v>
@@ -19622,7 +19625,7 @@
     </row>
     <row r="176" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -19723,7 +19726,7 @@
     </row>
     <row r="177" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -19824,7 +19827,7 @@
     </row>
     <row r="178" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -19925,7 +19928,7 @@
     </row>
     <row r="179" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -20026,7 +20029,7 @@
     </row>
     <row r="180" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -20127,7 +20130,7 @@
     </row>
     <row r="181" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -20236,14 +20239,14 @@
   <dimension ref="A1:AG81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1:AG81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1">
         <v>2019</v>
@@ -20344,7 +20347,7 @@
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A2" s="22" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B2" s="22">
         <v>35100000000000</v>
@@ -20445,7 +20448,7 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A3" s="22" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B3" s="22">
         <v>169300000000000</v>
@@ -20546,7 +20549,7 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A4" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B4" s="22">
         <v>16900000000000</v>
@@ -20647,7 +20650,7 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -20748,7 +20751,7 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A6" s="22" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B6" s="22">
         <v>58400000000000</v>
@@ -20849,7 +20852,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -20950,7 +20953,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -21051,7 +21054,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A9" s="22" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B9" s="22">
         <v>5700000000000</v>
@@ -21152,7 +21155,7 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A10" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B10" s="22">
         <v>400000000000</v>
@@ -21253,7 +21256,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -21354,7 +21357,7 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A12" s="22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B12" s="22">
         <v>170200000000000</v>
@@ -21455,7 +21458,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A13" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B13" s="22">
         <v>24000000000000</v>
@@ -21556,7 +21559,7 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A14" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B14" s="22">
         <v>4288000000000000</v>
@@ -21657,7 +21660,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A15" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B15" s="22">
         <v>902400000000000</v>
@@ -21758,7 +21761,7 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -21859,7 +21862,7 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -21960,7 +21963,7 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A18" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B18" s="22">
         <v>3.73448E+16</v>
@@ -22061,7 +22064,7 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -22162,7 +22165,7 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -22263,7 +22266,7 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -22364,7 +22367,7 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A22" s="22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B22" s="22">
         <v>210000000000000</v>
@@ -22465,7 +22468,7 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A23" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B23" s="22">
         <v>654300000000000</v>
@@ -22566,7 +22569,7 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A24" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B24" s="22">
         <v>432400000000000</v>
@@ -22667,7 +22670,7 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -22768,7 +22771,7 @@
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A26" s="22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B26" s="22">
         <v>2700000000000</v>
@@ -22869,7 +22872,7 @@
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -22970,7 +22973,7 @@
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -23071,7 +23074,7 @@
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A29" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B29" s="22">
         <v>21600000000000</v>
@@ -23172,7 +23175,7 @@
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A30" s="22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B30" s="22">
         <v>200000000000</v>
@@ -23273,7 +23276,7 @@
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -23374,7 +23377,7 @@
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A32" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B32" s="22">
         <v>424600000000000</v>
@@ -23475,7 +23478,7 @@
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A33" s="22" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B33" s="22">
         <v>44500000000000</v>
@@ -23576,7 +23579,7 @@
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A34" s="22" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B34" s="22">
         <v>3248000000000000</v>
@@ -23677,7 +23680,7 @@
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -23778,7 +23781,7 @@
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A36" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B36" s="22">
         <v>85500000000000</v>
@@ -23879,7 +23882,7 @@
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -23980,7 +23983,7 @@
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -24081,7 +24084,7 @@
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A39" s="22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B39" s="22">
         <v>161400000000000</v>
@@ -24182,7 +24185,7 @@
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A40" s="22" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B40" s="22">
         <v>3582300000000000</v>
@@ -24283,7 +24286,7 @@
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -24384,7 +24387,7 @@
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A42" s="22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B42" s="22">
         <v>83200000000000</v>
@@ -24485,7 +24488,7 @@
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A43" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B43" s="22">
         <v>79900000000000</v>
@@ -24586,7 +24589,7 @@
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A44" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B44" s="22">
         <v>58700000000000</v>
@@ -24687,7 +24690,7 @@
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -24788,7 +24791,7 @@
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A46" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B46" s="22">
         <v>48690000000000</v>
@@ -24889,7 +24892,7 @@
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -24990,7 +24993,7 @@
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -25091,7 +25094,7 @@
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A49" s="22" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B49" s="22">
         <v>11633500000000</v>
@@ -25192,7 +25195,7 @@
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -25293,7 +25296,7 @@
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -25394,7 +25397,7 @@
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A52" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B52" s="22">
         <v>222600000000000</v>
@@ -25495,7 +25498,7 @@
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -25596,7 +25599,7 @@
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -25697,7 +25700,7 @@
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -25798,7 +25801,7 @@
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -25899,7 +25902,7 @@
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -26000,7 +26003,7 @@
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -26101,7 +26104,7 @@
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -26202,7 +26205,7 @@
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -26303,7 +26306,7 @@
     </row>
     <row r="61" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -26404,7 +26407,7 @@
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A62" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B62" s="22">
         <v>256600000000000</v>
@@ -26505,7 +26508,7 @@
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -26606,7 +26609,7 @@
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A64" s="22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B64" s="22">
         <v>179500000000000</v>
@@ -26707,7 +26710,7 @@
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -26808,7 +26811,7 @@
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A66" s="22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B66" s="22">
         <v>522900000000000</v>
@@ -26909,7 +26912,7 @@
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -27010,7 +27013,7 @@
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -27111,7 +27114,7 @@
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A69" s="22" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B69" s="22">
         <v>51500000000000</v>
@@ -27212,7 +27215,7 @@
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A70" s="22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B70" s="22">
         <v>85500000000000</v>
@@ -27313,7 +27316,7 @@
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -27414,7 +27417,7 @@
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A72" s="22" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B72" s="22">
         <v>1829000000000000</v>
@@ -27515,7 +27518,7 @@
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A73" s="22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B73" s="22">
         <v>142000000000000</v>
@@ -27616,7 +27619,7 @@
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A74" s="22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B74" s="22">
         <v>3010000000000000</v>
@@ -27717,7 +27720,7 @@
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -27818,7 +27821,7 @@
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A76" s="22" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B76" s="22">
         <v>2265000000000000</v>
@@ -27919,7 +27922,7 @@
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -28020,7 +28023,7 @@
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -28121,7 +28124,7 @@
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A79" s="22" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B79" s="22">
         <v>197617000000000</v>
@@ -28222,7 +28225,7 @@
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A80" s="22" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B80" s="22">
         <v>91600000000000</v>
@@ -28323,7 +28326,7 @@
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -28431,7 +28434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -28449,7 +28452,7 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="F1" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -28457,25 +28460,25 @@
     </row>
     <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="D2" s="19" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="I2" s="19" t="s">
         <v>6</v>
@@ -28489,11 +28492,11 @@
         <v>1429</v>
       </c>
       <c r="C3">
-        <v>1435</v>
+        <v>1485</v>
       </c>
       <c r="D3">
         <f>(C3-B3)/B3</f>
-        <v>4.1987403778866337E-3</v>
+        <v>3.9188243526941918E-2</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
@@ -28502,11 +28505,11 @@
         <v>13.77</v>
       </c>
       <c r="H3">
-        <v>12.77</v>
+        <v>12.92</v>
       </c>
       <c r="I3">
         <f>(H3-G3)/G3</f>
-        <v>-7.2621641249092234E-2</v>
+        <v>-6.1728395061728371E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -28517,11 +28520,11 @@
         <v>1355</v>
       </c>
       <c r="C4">
-        <v>1260</v>
+        <v>1268</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D6" si="0">(C4-B4)/B4</f>
-        <v>-7.0110701107011064E-2</v>
+        <v>-6.4206642066420669E-2</v>
       </c>
       <c r="F4" t="s">
         <v>35</v>
@@ -28530,11 +28533,11 @@
         <v>9.4600000000000009</v>
       </c>
       <c r="H4">
-        <v>9</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I5" si="1">(H4-G4)/G4</f>
-        <v>-4.8625792811839409E-2</v>
+        <v>-6.9767441860465129E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -28545,11 +28548,11 @@
         <v>946</v>
       </c>
       <c r="C5">
-        <v>899</v>
+        <v>895</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>-4.9682875264270614E-2</v>
+        <v>-5.3911205073995772E-2</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
@@ -28558,11 +28561,11 @@
         <v>24.19</v>
       </c>
       <c r="H5">
-        <v>21.55</v>
+        <v>21.95</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>-0.10913600661430345</v>
+        <v>-9.2600248036378743E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -28573,11 +28576,11 @@
         <v>3885</v>
       </c>
       <c r="C6">
-        <v>3730</v>
+        <v>3802</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-3.9897039897039896E-2</v>
+        <v>-2.1364221364221364E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -28588,7 +28591,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="F8" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -28596,22 +28599,22 @@
     </row>
     <row r="9" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="B9" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>6</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G9" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>45</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>6</v>
@@ -28625,39 +28628,39 @@
         <v>9015</v>
       </c>
       <c r="C10">
-        <v>7931</v>
+        <v>7874</v>
       </c>
       <c r="D10">
         <f>(C10-B10)/B10</f>
-        <v>-0.12024403771491958</v>
+        <v>-0.12656683305601774</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10">
         <v>0.7</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="I10">
         <f>(H10-G10)/G10</f>
-        <v>0.42857142857142866</v>
+        <v>0.28571428571428581</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="F11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G11">
         <v>28.6</v>
       </c>
       <c r="H11">
-        <v>26.3</v>
+        <v>25.9</v>
       </c>
       <c r="I11">
         <f>(H11-G11)/G11</f>
-        <v>-8.0419580419580444E-2</v>
+        <v>-9.4405594405594498E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -28668,11 +28671,11 @@
         <v>19448</v>
       </c>
       <c r="C12">
-        <v>17517</v>
+        <v>18168</v>
       </c>
       <c r="D12">
         <f>(C12-B12)/B12</f>
-        <v>-9.9290415466886051E-2</v>
+        <v>-6.5816536404771697E-2</v>
       </c>
     </row>
   </sheetData>
@@ -28708,7 +28711,7 @@
       </c>
       <c r="B2" s="7">
         <f>Calculations!E28</f>
-        <v>1.2110336848678172</v>
+        <v>1.9230248197448696</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -28717,7 +28720,7 @@
       </c>
       <c r="B3" s="14">
         <f>Calculations!F28</f>
-        <v>0.40182166334419034</v>
+        <v>0.32460263835263836</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -28726,7 +28729,7 @@
       </c>
       <c r="B4" s="7">
         <f>Calculations!B28</f>
-        <v>0.35611595920953071</v>
+        <v>0.1941373502873644</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -28735,7 +28738,7 @@
       </c>
       <c r="B5" s="7">
         <f>Calculations!C28</f>
-        <v>0.61077939841578666</v>
+        <v>1.0094071850405399</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -28744,7 +28747,7 @@
       </c>
       <c r="B6" s="7">
         <f>Calculations!D28</f>
-        <v>0.76655174860418485</v>
+        <v>1.3083596617483817</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Update COVID recession data
Updated to November STEO and CBO recovery projections
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
+++ b/InputData/ctrl-settings/EoSEUwGDPiR/Elasticity of Sectoral Energy Use wrt Per Capita GDP in Recession.xlsx
@@ -1692,7 +1692,7 @@
       </c>
       <c r="C4">
         <f>EIA!D5</f>
-        <v>-5.3911205073995772E-2</v>
+        <v>-3.382663847780127E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
@@ -1705,7 +1705,7 @@
       </c>
       <c r="C5">
         <f>EIA!I5</f>
-        <v>-9.2600248036378743E-2</v>
+        <v>-6.9450186027283992E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -1718,7 +1718,7 @@
       </c>
       <c r="C6">
         <f>EIA!I11</f>
-        <v>-9.4405594405594498E-2</v>
+        <v>-0.11888111888111895</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="C9">
         <f>EIA!D3</f>
-        <v>3.9188243526941918E-2</v>
+        <v>3.2890132960111965E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -1760,7 +1760,7 @@
       </c>
       <c r="C11">
         <f>EIA!I3</f>
-        <v>-6.1728395061728371E-2</v>
+        <v>-4.3572984749455312E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C14">
         <f>EIA!D4</f>
-        <v>-6.4206642066420669E-2</v>
+        <v>-5.9778597785977862E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
@@ -1803,7 +1803,7 @@
       </c>
       <c r="C16">
         <f>EIA!I4</f>
-        <v>-6.9767441860465129E-2</v>
+        <v>-7.3995771670190377E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -1835,13 +1835,13 @@
       </c>
       <c r="C20">
         <f>EIA!C12</f>
-        <v>18168</v>
+        <v>18411</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="16">
         <f>-(1-C20/B20)</f>
-        <v>-6.5816536404771697E-2</v>
+        <v>-5.3321678321678334E-2</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>30</v>
@@ -1879,23 +1879,23 @@
       </c>
       <c r="B26" s="6">
         <f>SUMPRODUCT(B9:B11,C9:C11)/SUM(B9:B11)</f>
-        <v>-1.2777447982714234E-2</v>
+        <v>-6.4835406216792509E-3</v>
       </c>
       <c r="C26" s="6">
         <f>SUMPRODUCT(B14:B16,C14:C16)/SUM(B14:B16)</f>
-        <v>-6.643568474145882E-2</v>
+        <v>-6.5757673833730559E-2</v>
       </c>
       <c r="D26" s="6">
         <f>SUMPRODUCT(B4:B6,C4:C6)/SUM(B4:B6)</f>
-        <v>-8.6111701307997141E-2</v>
+        <v>-9.844646725351093E-2</v>
       </c>
       <c r="E26" s="6">
         <f>(EIA!C10-EIA!B10)/EIA!B10</f>
-        <v>-0.12656683305601774</v>
+        <v>-0.13455352190793124</v>
       </c>
       <c r="F26" s="13">
         <f>(EIA!C6-EIA!B6)/EIA!B6</f>
-        <v>-2.1364221364221364E-2</v>
+        <v>-1.8532818532818532E-2</v>
       </c>
       <c r="G26" s="24"/>
     </row>
@@ -1909,23 +1909,23 @@
       </c>
       <c r="B28" s="11">
         <f>B26/$A$22</f>
-        <v>0.1941373502873644</v>
+        <v>0.12159295854427969</v>
       </c>
       <c r="C28" s="11">
         <f>C26/$A$22</f>
-        <v>1.0094071850405399</v>
+        <v>1.2332258830457008</v>
       </c>
       <c r="D28" s="11">
         <f>D26/$A$22</f>
-        <v>1.3083596617483817</v>
+        <v>1.8462747301314177</v>
       </c>
       <c r="E28" s="11">
         <f>E26/$A$22</f>
-        <v>1.9230248197448696</v>
+        <v>2.5234299846339887</v>
       </c>
       <c r="F28" s="11">
         <f>F26/$A$22</f>
-        <v>0.32460263835263836</v>
+        <v>0.34756630166466224</v>
       </c>
       <c r="G28" s="14"/>
     </row>
@@ -1939,7 +1939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG181"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:AG181"/>
     </sheetView>
   </sheetViews>
@@ -28492,11 +28492,11 @@
         <v>1429</v>
       </c>
       <c r="C3">
-        <v>1485</v>
+        <v>1476</v>
       </c>
       <c r="D3">
         <f>(C3-B3)/B3</f>
-        <v>3.9188243526941918E-2</v>
+        <v>3.2890132960111965E-2</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
@@ -28505,11 +28505,11 @@
         <v>13.77</v>
       </c>
       <c r="H3">
-        <v>12.92</v>
+        <v>13.17</v>
       </c>
       <c r="I3">
         <f>(H3-G3)/G3</f>
-        <v>-6.1728395061728371E-2</v>
+        <v>-4.3572984749455312E-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -28520,11 +28520,11 @@
         <v>1355</v>
       </c>
       <c r="C4">
-        <v>1268</v>
+        <v>1274</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D6" si="0">(C4-B4)/B4</f>
-        <v>-6.4206642066420669E-2</v>
+        <v>-5.9778597785977862E-2</v>
       </c>
       <c r="F4" t="s">
         <v>35</v>
@@ -28533,11 +28533,11 @@
         <v>9.4600000000000009</v>
       </c>
       <c r="H4">
-        <v>8.8000000000000007</v>
+        <v>8.76</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I5" si="1">(H4-G4)/G4</f>
-        <v>-6.9767441860465129E-2</v>
+        <v>-7.3995771670190377E-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -28548,11 +28548,11 @@
         <v>946</v>
       </c>
       <c r="C5">
-        <v>895</v>
+        <v>914</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>-5.3911205073995772E-2</v>
+        <v>-3.382663847780127E-2</v>
       </c>
       <c r="F5" t="s">
         <v>36</v>
@@ -28561,11 +28561,11 @@
         <v>24.19</v>
       </c>
       <c r="H5">
-        <v>21.95</v>
+        <v>22.51</v>
       </c>
       <c r="I5">
         <f t="shared" si="1"/>
-        <v>-9.2600248036378743E-2</v>
+        <v>-6.9450186027283992E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -28576,11 +28576,11 @@
         <v>3885</v>
       </c>
       <c r="C6">
-        <v>3802</v>
+        <v>3813</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>-2.1364221364221364E-2</v>
+        <v>-1.8532818532818532E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -28628,11 +28628,11 @@
         <v>9015</v>
       </c>
       <c r="C10">
-        <v>7874</v>
+        <v>7802</v>
       </c>
       <c r="D10">
         <f>(C10-B10)/B10</f>
-        <v>-0.12656683305601774</v>
+        <v>-0.13455352190793124</v>
       </c>
       <c r="F10" t="s">
         <v>54</v>
@@ -28656,11 +28656,11 @@
         <v>28.6</v>
       </c>
       <c r="H11">
-        <v>25.9</v>
+        <v>25.2</v>
       </c>
       <c r="I11">
         <f>(H11-G11)/G11</f>
-        <v>-9.4405594405594498E-2</v>
+        <v>-0.11888111888111895</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -28671,11 +28671,11 @@
         <v>19448</v>
       </c>
       <c r="C12">
-        <v>18168</v>
+        <v>18411</v>
       </c>
       <c r="D12">
         <f>(C12-B12)/B12</f>
-        <v>-6.5816536404771697E-2</v>
+        <v>-5.332167832167832E-2</v>
       </c>
     </row>
   </sheetData>
@@ -28711,7 +28711,7 @@
       </c>
       <c r="B2" s="7">
         <f>Calculations!E28</f>
-        <v>1.9230248197448696</v>
+        <v>2.5234299846339887</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -28720,7 +28720,7 @@
       </c>
       <c r="B3" s="14">
         <f>Calculations!F28</f>
-        <v>0.32460263835263836</v>
+        <v>0.34756630166466224</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -28729,7 +28729,7 @@
       </c>
       <c r="B4" s="7">
         <f>Calculations!B28</f>
-        <v>0.1941373502873644</v>
+        <v>0.12159295854427969</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -28738,7 +28738,7 @@
       </c>
       <c r="B5" s="7">
         <f>Calculations!C28</f>
-        <v>1.0094071850405399</v>
+        <v>1.2332258830457008</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -28747,7 +28747,7 @@
       </c>
       <c r="B6" s="7">
         <f>Calculations!D28</f>
-        <v>1.3083596617483817</v>
+        <v>1.8462747301314177</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>